<commit_message>
added a pandas time series example to data notebook
</commit_message>
<xml_diff>
--- a/module 1 - data/temperature_data.xlsx
+++ b/module 1 - data/temperature_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -362,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,7 +378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -386,7 +386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -394,7 +394,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -402,11 +402,16 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>30</v>
       </c>
     </row>
@@ -417,15 +422,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -441,7 +446,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -449,7 +454,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -457,11 +462,16 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>29.2</v>
       </c>
     </row>

</xml_diff>